<commit_message>
Solder Kit Instructions Update
</commit_message>
<xml_diff>
--- a/Solder Kits/intro-to-solder-kit-v1/misc files/intro-to-solder-kit-v1-bom.xlsx
+++ b/Solder Kits/intro-to-solder-kit-v1/misc files/intro-to-solder-kit-v1-bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0C1709-1D41-4BA2-8784-F9CCFE6472FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB760597-71F3-4B05-A851-E8EADB9FB118}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="3630" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="2775" windowWidth="21555" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>PCB</t>
   </si>
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t>https://www.amazon.com/gp/product/B077XDC3ZN/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1</t>
-  </si>
-  <si>
-    <t>Badge Magnet</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Set-100-Magnetics-Neodymium-BM-2MAG-1/dp/B00CI9XKVC/ref=sr_1_35?keywords=badge+magnet&amp;qid=1552090999&amp;s=gateway&amp;sr=8-35</t>
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/keystone-electronics/3035/36-3035-ND/5872907</t>
@@ -425,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +457,7 @@
         <v>0.875</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D7" si="0">C2*A2</f>
+        <f t="shared" ref="D2:D6" si="0">C2*A2</f>
         <v>0.875</v>
       </c>
     </row>
@@ -482,7 +476,7 @@
         <v>0.22</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -538,34 +532,16 @@
         <v>0.12</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2">
-        <f>SUM(D2:D7)</f>
-        <v>2.3250000000000002</v>
+      <c r="D7" s="2">
+        <f>SUM(D2:D6)</f>
+        <v>1.9750000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>